<commit_message>
add SECONDARY_RES to RRL archetypes
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/CH_ReMaP/archetypes/RRL_2040_BAU/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/remap_ville_plugin/CH_ReMaP/archetypes/RRL_2040_BAU/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shsieh\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\RRL_2040_BAU\use_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C596164C-1DFF-4B0C-AC9E-F0A17BACA3A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492C5F21-590B-4A4D-9C58-6A8B42AB4EC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19260" yWindow="2190" windowWidth="14400" windowHeight="10890" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="INTERNAL_LOADS" sheetId="1" r:id="rId1"/>
-    <sheet name="INDOOR_COMFORT" sheetId="2" r:id="rId2"/>
+    <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId1"/>
+    <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -27,131 +30,137 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+  <si>
+    <t>Ths_set_C</t>
+  </si>
+  <si>
+    <t>Ea_Wm2</t>
+  </si>
+  <si>
+    <t>El_Wm2</t>
+  </si>
+  <si>
+    <t>Epro_Wm2</t>
+  </si>
+  <si>
+    <t>Tcs_set_C</t>
+  </si>
+  <si>
+    <t>MULTI_RES</t>
+  </si>
+  <si>
+    <t>SINGLE_RES</t>
+  </si>
+  <si>
+    <t>HOTEL</t>
+  </si>
+  <si>
+    <t>OFFICE</t>
+  </si>
+  <si>
+    <t>RETAIL</t>
+  </si>
+  <si>
+    <t>RESTAURANT</t>
+  </si>
+  <si>
+    <t>INDUSTRIAL</t>
+  </si>
+  <si>
+    <t>SCHOOL</t>
+  </si>
+  <si>
+    <t>HOSPITAL</t>
+  </si>
+  <si>
+    <t>GYM</t>
+  </si>
+  <si>
+    <t>SWIMMING</t>
+  </si>
+  <si>
+    <t>SERVERROOM</t>
+  </si>
+  <si>
+    <t>PARKING</t>
+  </si>
+  <si>
+    <t>COOLROOM</t>
+  </si>
+  <si>
+    <t>FOODSTORE</t>
+  </si>
+  <si>
+    <t>Ed_Wm2</t>
+  </si>
+  <si>
+    <t>Tcs_setb_C</t>
+  </si>
+  <si>
+    <t>Ths_setb_C</t>
+  </si>
+  <si>
+    <t>LAB</t>
+  </si>
+  <si>
+    <t>MUSEUM</t>
+  </si>
+  <si>
+    <t>LIBRARY</t>
+  </si>
+  <si>
+    <t>Qhpro_Wm2</t>
+  </si>
+  <si>
+    <t>Qcre_Wm2</t>
+  </si>
+  <si>
+    <t>UNIVERSITY</t>
+  </si>
+  <si>
+    <t>Qcpro_Wm2</t>
+  </si>
+  <si>
+    <t>RH_min_pc</t>
+  </si>
+  <si>
+    <t>RH_max_pc</t>
+  </si>
   <si>
     <t>code</t>
   </si>
   <si>
+    <t>Ev_kWveh</t>
+  </si>
+  <si>
+    <t>Vww_ldp</t>
+  </si>
+  <si>
+    <t>Vw_ldp</t>
+  </si>
+  <si>
+    <t>X_ghp</t>
+  </si>
+  <si>
+    <t>Qs_Wp</t>
+  </si>
+  <si>
     <t>Occ_m2p</t>
   </si>
   <si>
-    <t>Qs_Wp</t>
-  </si>
-  <si>
-    <t>X_ghp</t>
-  </si>
-  <si>
-    <t>Ea_Wm2</t>
-  </si>
-  <si>
-    <t>El_Wm2</t>
-  </si>
-  <si>
-    <t>Epro_Wm2</t>
-  </si>
-  <si>
-    <t>Ed_Wm2</t>
-  </si>
-  <si>
-    <t>Vww_ldp</t>
-  </si>
-  <si>
-    <t>Vw_ldp</t>
-  </si>
-  <si>
-    <t>Qcre_Wm2</t>
-  </si>
-  <si>
-    <t>Qhpro_Wm2</t>
-  </si>
-  <si>
-    <t>Qcpro_Wm2</t>
-  </si>
-  <si>
-    <t>Ev_kWveh</t>
-  </si>
-  <si>
-    <t>MULTI_RES</t>
-  </si>
-  <si>
-    <t>SINGLE_RES</t>
-  </si>
-  <si>
-    <t>HOTEL</t>
-  </si>
-  <si>
-    <t>OFFICE</t>
-  </si>
-  <si>
-    <t>RETAIL</t>
-  </si>
-  <si>
-    <t>FOODSTORE</t>
-  </si>
-  <si>
-    <t>RESTAURANT</t>
-  </si>
-  <si>
-    <t>INDUSTRIAL</t>
-  </si>
-  <si>
-    <t>SCHOOL</t>
-  </si>
-  <si>
-    <t>HOSPITAL</t>
-  </si>
-  <si>
-    <t>GYM</t>
-  </si>
-  <si>
-    <t>SWIMMING</t>
-  </si>
-  <si>
-    <t>SERVERROOM</t>
-  </si>
-  <si>
-    <t>PARKING</t>
-  </si>
-  <si>
-    <t>COOLROOM</t>
-  </si>
-  <si>
-    <t>LAB</t>
-  </si>
-  <si>
-    <t>MUSEUM</t>
-  </si>
-  <si>
-    <t>LIBRARY</t>
-  </si>
-  <si>
-    <t>UNIVERSITY</t>
-  </si>
-  <si>
-    <t>Tcs_set_C</t>
-  </si>
-  <si>
-    <t>Ths_set_C</t>
-  </si>
-  <si>
-    <t>Tcs_setb_C</t>
-  </si>
-  <si>
-    <t>Ths_setb_C</t>
-  </si>
-  <si>
     <t>Ve_lsp</t>
   </si>
   <si>
-    <t>RH_min_pc</t>
-  </si>
-  <si>
-    <t>RH_max_pc</t>
+    <t>SECONDARY_RES</t>
   </si>
 </sst>
 </file>
@@ -161,8 +170,128 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -177,12 +306,185 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -197,12 +499,119 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -234,41 +643,123 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -546,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,69 +1048,68 @@
     <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.453125" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.1796875" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="1"/>
+    <col min="11" max="11" width="12.6328125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B2" s="9">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C2" s="9">
         <v>70</v>
@@ -660,10 +1150,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B3" s="9">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="C3" s="7">
         <v>70</v>
@@ -703,22 +1193,22 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>16</v>
+      <c r="A4" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="B4" s="9">
-        <v>15</v>
-      </c>
-      <c r="C4" s="9">
+        <v>60</v>
+      </c>
+      <c r="C4" s="7">
         <v>70</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>80</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>8</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>2.7</v>
       </c>
       <c r="G4" s="9">
@@ -747,11 +1237,11 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>17</v>
+      <c r="A5" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="9">
         <v>70</v>
@@ -760,10 +1250,10 @@
         <v>80</v>
       </c>
       <c r="E5" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="9">
-        <v>15.9</v>
+        <v>2.7</v>
       </c>
       <c r="G5" s="9">
         <v>0</v>
@@ -772,10 +1262,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="9">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="J5" s="9">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="K5" s="7">
         <v>0</v>
@@ -792,10 +1282,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B6" s="9">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" s="9">
         <v>70</v>
@@ -804,115 +1294,115 @@
         <v>80</v>
       </c>
       <c r="E6" s="9">
+        <v>7</v>
+      </c>
+      <c r="F6" s="9">
+        <v>15.9</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9">
+        <v>3</v>
+      </c>
+      <c r="J6" s="9">
+        <v>60</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9">
+        <v>70</v>
+      </c>
+      <c r="D7" s="9">
+        <v>80</v>
+      </c>
+      <c r="E7" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F7" s="9">
         <f>9.3+24</f>
         <v>33.299999999999997</v>
       </c>
-      <c r="G6" s="9">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
         <v>2</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J7" s="9">
         <v>30</v>
       </c>
-      <c r="K6" s="7">
-        <v>0</v>
-      </c>
-      <c r="L6" s="7">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7">
-        <v>0</v>
-      </c>
-      <c r="N6" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B8" s="9">
         <v>8</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C8" s="9">
         <v>70</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D8" s="9">
         <v>80</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E8" s="9">
         <v>2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F8" s="9">
         <f>9.3+12</f>
         <v>21.3</v>
       </c>
-      <c r="G7" s="9">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
         <v>2</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J8" s="9">
         <v>30</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K8" s="7">
         <v>10</v>
-      </c>
-      <c r="L7" s="7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7">
-        <v>0</v>
-      </c>
-      <c r="N7" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="9">
-        <v>2</v>
-      </c>
-      <c r="C8" s="9">
-        <v>70</v>
-      </c>
-      <c r="D8" s="9">
-        <v>80</v>
-      </c>
-      <c r="E8" s="9">
-        <v>2</v>
-      </c>
-      <c r="F8" s="9">
-        <v>6.9</v>
-      </c>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
-        <v>15</v>
-      </c>
-      <c r="J8" s="9">
-        <v>45</v>
-      </c>
-      <c r="K8" s="7">
-        <v>0</v>
       </c>
       <c r="L8" s="7">
         <v>0</v>
@@ -926,40 +1416,40 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B9" s="9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9">
+        <v>70</v>
+      </c>
+      <c r="D9" s="9">
+        <v>80</v>
+      </c>
+      <c r="E9" s="9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9">
+        <v>6.9</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
         <v>15</v>
       </c>
-      <c r="C9" s="9">
-        <v>90</v>
-      </c>
-      <c r="D9" s="9">
-        <v>170</v>
-      </c>
-      <c r="E9" s="9">
-        <v>10</v>
-      </c>
-      <c r="F9" s="9">
-        <v>10.8</v>
-      </c>
-      <c r="G9" s="9">
-        <v>16.5</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
-        <v>3</v>
-      </c>
       <c r="J9" s="9">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="K9" s="7">
         <v>0</v>
       </c>
       <c r="L9" s="7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="M9" s="7">
         <v>0</v>
@@ -970,40 +1460,40 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B10" s="9">
+        <v>15</v>
+      </c>
+      <c r="C10" s="9">
+        <v>90</v>
+      </c>
+      <c r="D10" s="9">
+        <v>170</v>
+      </c>
+      <c r="E10" s="9">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9">
+        <v>10.8</v>
+      </c>
+      <c r="G10" s="9">
+        <v>16.5</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9">
         <v>3</v>
       </c>
-      <c r="C10" s="9">
-        <v>70</v>
-      </c>
-      <c r="D10" s="9">
-        <v>80</v>
-      </c>
-      <c r="E10" s="9">
-        <v>4</v>
-      </c>
-      <c r="F10" s="9">
-        <v>14</v>
-      </c>
-      <c r="G10" s="9">
-        <v>0</v>
-      </c>
-      <c r="H10" s="7">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
-        <v>2</v>
-      </c>
       <c r="J10" s="9">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K10" s="7">
         <v>0</v>
       </c>
       <c r="L10" s="7">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="M10" s="7">
         <v>0</v>
@@ -1014,89 +1504,89 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B11" s="9">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9">
+        <v>70</v>
+      </c>
+      <c r="D11" s="9">
+        <v>80</v>
+      </c>
+      <c r="E11" s="9">
+        <v>4</v>
+      </c>
+      <c r="F11" s="9">
+        <v>14</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>2</v>
+      </c>
+      <c r="J11" s="9">
+        <v>30</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="9">
         <f>15*0.43+3*0.01+5*0.56</f>
         <v>9.2800000000000011</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C12" s="9">
         <v>70</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D12" s="9">
         <v>80</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E12" s="9">
         <f>0.43*4+0.01*7+0.56*20</f>
         <v>12.990000000000002</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F12" s="9">
         <f>0.43*4.5+0.01*15.9+0.56*15.9</f>
         <v>10.998000000000001</v>
       </c>
-      <c r="G11" s="9">
-        <v>0</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
-      <c r="I11" s="9">
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9">
         <f>0.43*60+0.01*0+0.56*0</f>
         <v>25.8</v>
       </c>
-      <c r="J11" s="9">
-        <f>I11*4</f>
+      <c r="J12" s="9">
+        <f>I12*4</f>
         <v>103.2</v>
       </c>
-      <c r="K11" s="7">
-        <v>0</v>
-      </c>
-      <c r="L11" s="7">
+      <c r="K12" s="7">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7">
         <v>16</v>
-      </c>
-      <c r="M11" s="7">
-        <v>0</v>
-      </c>
-      <c r="N11" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="9">
-        <v>10</v>
-      </c>
-      <c r="C12" s="9">
-        <v>120</v>
-      </c>
-      <c r="D12" s="9">
-        <v>280</v>
-      </c>
-      <c r="E12" s="9">
-        <v>2</v>
-      </c>
-      <c r="F12" s="9">
-        <v>9.9</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="H12" s="7">
-        <v>0</v>
-      </c>
-      <c r="I12" s="9">
-        <v>60</v>
-      </c>
-      <c r="J12" s="9">
-        <v>180</v>
-      </c>
-      <c r="K12" s="7">
-        <v>0</v>
-      </c>
-      <c r="L12" s="7">
-        <v>0</v>
       </c>
       <c r="M12" s="7">
         <v>0</v>
@@ -1107,22 +1597,22 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B13" s="9">
         <v>10</v>
       </c>
       <c r="C13" s="9">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D13" s="9">
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="E13" s="9">
         <v>2</v>
       </c>
       <c r="F13" s="9">
-        <v>11.3</v>
+        <v>9.9</v>
       </c>
       <c r="G13" s="9">
         <v>0</v>
@@ -1131,10 +1621,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="9">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="J13" s="9">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="K13" s="7">
         <v>0</v>
@@ -1151,34 +1641,34 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B14" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C14" s="9">
         <v>70</v>
       </c>
       <c r="D14" s="9">
-        <v>0</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2</v>
       </c>
       <c r="F14" s="9">
-        <v>6.6</v>
+        <v>11.3</v>
       </c>
       <c r="G14" s="9">
         <v>0</v>
       </c>
-      <c r="H14" s="9">
-        <v>100</v>
+      <c r="H14" s="7">
+        <v>0</v>
       </c>
       <c r="I14" s="9">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J14" s="9">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="K14" s="7">
         <v>0</v>
@@ -1195,28 +1685,28 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B15" s="9">
         <v>0</v>
       </c>
       <c r="C15" s="9">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D15" s="9">
         <v>0</v>
       </c>
-      <c r="E15" s="9">
-        <v>1</v>
+      <c r="E15" s="8">
+        <v>0</v>
       </c>
       <c r="F15" s="9">
-        <v>2.9</v>
+        <v>6.6</v>
       </c>
       <c r="G15" s="9">
         <v>0</v>
       </c>
-      <c r="H15" s="7">
-        <v>0</v>
+      <c r="H15" s="9">
+        <v>100</v>
       </c>
       <c r="I15" s="9">
         <v>0</v>
@@ -1239,22 +1729,22 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B16" s="9">
         <v>0</v>
       </c>
       <c r="C16" s="9">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="D16" s="9">
         <v>0</v>
       </c>
       <c r="E16" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="9">
-        <v>5.7</v>
+        <v>2.9</v>
       </c>
       <c r="G16" s="9">
         <v>0</v>
@@ -1269,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L16" s="7">
         <v>0</v>
@@ -1283,40 +1773,37 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B17" s="9">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C17" s="9">
-        <f>C11</f>
         <v>70</v>
       </c>
       <c r="D17" s="9">
-        <f>D11</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E17" s="9">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F17" s="9">
-        <v>16.2</v>
+        <v>5.7</v>
       </c>
       <c r="G17" s="9">
-        <f>G9</f>
-        <v>16.5</v>
+        <v>0</v>
       </c>
       <c r="H17" s="7">
         <v>0</v>
       </c>
       <c r="I17" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J17" s="9">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K17" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L17" s="7">
         <v>0</v>
@@ -1330,34 +1817,37 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B18" s="9">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9">
+        <f>C12</f>
+        <v>70</v>
+      </c>
+      <c r="D18" s="9">
+        <f>D12</f>
+        <v>80</v>
+      </c>
+      <c r="E18" s="9">
+        <v>20</v>
+      </c>
+      <c r="F18" s="9">
+        <v>16.2</v>
+      </c>
+      <c r="G18" s="9">
+        <f>G10</f>
+        <v>16.5</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="9">
         <v>3</v>
       </c>
-      <c r="C18" s="9">
-        <v>70</v>
-      </c>
-      <c r="D18" s="9">
-        <v>80</v>
-      </c>
-      <c r="E18" s="9">
-        <v>7</v>
-      </c>
-      <c r="F18" s="9">
-        <v>10.8</v>
-      </c>
-      <c r="G18" s="9">
-        <v>0</v>
-      </c>
-      <c r="H18" s="7">
-        <v>0</v>
-      </c>
-      <c r="I18" s="9">
-        <v>2</v>
-      </c>
       <c r="J18" s="9">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K18" s="7">
         <v>0</v>
@@ -1374,10 +1864,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B19" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" s="9">
         <v>70</v>
@@ -1386,22 +1876,22 @@
         <v>80</v>
       </c>
       <c r="E19" s="9">
+        <v>7</v>
+      </c>
+      <c r="F19" s="9">
+        <v>10.8</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0</v>
+      </c>
+      <c r="I19" s="9">
         <v>2</v>
       </c>
-      <c r="F19" s="9">
-        <v>6.9</v>
-      </c>
-      <c r="G19" s="9">
-        <v>0</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0</v>
-      </c>
-      <c r="I19" s="9">
-        <v>0</v>
-      </c>
       <c r="J19" s="9">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K19" s="7">
         <v>0</v>
@@ -1418,10 +1908,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B20" s="9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C20" s="9">
         <v>70</v>
@@ -1430,48 +1920,92 @@
         <v>80</v>
       </c>
       <c r="E20" s="9">
+        <v>2</v>
+      </c>
+      <c r="F20" s="9">
+        <v>6.9</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7">
+        <v>0</v>
+      </c>
+      <c r="I20" s="9">
+        <v>0</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+      <c r="L20" s="7">
+        <v>0</v>
+      </c>
+      <c r="M20" s="7">
+        <v>0</v>
+      </c>
+      <c r="N20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="9">
+        <v>10</v>
+      </c>
+      <c r="C21" s="9">
+        <v>70</v>
+      </c>
+      <c r="D21" s="9">
+        <v>80</v>
+      </c>
+      <c r="E21" s="9">
         <v>4</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F21" s="9">
         <v>12.5</v>
       </c>
-      <c r="G20" s="9">
-        <v>0</v>
-      </c>
-      <c r="H20" s="7">
-        <v>0</v>
-      </c>
-      <c r="I20" s="9">
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0</v>
+      </c>
+      <c r="I21" s="9">
         <v>2</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J21" s="9">
         <v>30</v>
       </c>
-      <c r="K20" s="7">
-        <v>0</v>
-      </c>
-      <c r="L20" s="7">
-        <v>0</v>
-      </c>
-      <c r="M20" s="7">
-        <v>0</v>
-      </c>
-      <c r="N20" s="7">
+      <c r="K21" s="7">
+        <v>0</v>
+      </c>
+      <c r="L21" s="7">
+        <v>0</v>
+      </c>
+      <c r="M21" s="7">
+        <v>0</v>
+      </c>
+      <c r="N21" s="7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1484,39 +2018,38 @@
     <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>26</v>
@@ -1531,7 +2064,8 @@
         <v>18</v>
       </c>
       <c r="F2" s="7">
-        <v>8.3000000000000007</v>
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="G2" s="7">
         <v>30</v>
@@ -1542,7 +2076,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>26</v>
@@ -1568,8 +2102,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>16</v>
+      <c r="A4" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="B4" s="2">
         <v>26</v>
@@ -1581,11 +2115,11 @@
         <v>28</v>
       </c>
       <c r="E4" s="4">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F4" s="7">
-        <f>36/3.6</f>
-        <v>10</v>
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="G4" s="7">
         <v>30</v>
@@ -1596,7 +2130,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>26</v>
@@ -1608,7 +2142,7 @@
         <v>28</v>
       </c>
       <c r="E5" s="4">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F5" s="7">
         <f>36/3.6</f>
@@ -1622,14 +2156,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
+      <c r="A6" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>26</v>
       </c>
       <c r="C6" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2">
         <v>28</v>
@@ -1638,8 +2172,8 @@
         <v>12</v>
       </c>
       <c r="F6" s="7">
-        <f>30/3.6</f>
-        <v>8.3333333333333339</v>
+        <f>36/3.6</f>
+        <v>10</v>
       </c>
       <c r="G6" s="7">
         <v>30</v>
@@ -1650,7 +2184,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>26</v>
@@ -1677,13 +2211,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
         <v>26</v>
       </c>
       <c r="C8" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2">
         <v>28</v>
@@ -1692,183 +2226,184 @@
         <v>12</v>
       </c>
       <c r="F8" s="7">
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="G8" s="7">
+        <v>30</v>
+      </c>
+      <c r="H8" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4">
+        <v>12</v>
+      </c>
+      <c r="F9" s="7">
         <f>36/3.6</f>
         <v>10</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G9" s="7">
         <v>30</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H9" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
         <v>30</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C10" s="4">
         <v>18</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="2">
         <v>32</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E10" s="4">
         <v>12</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F10" s="7">
         <f>10*15/3.6</f>
         <v>41.666666666666664</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G10" s="7">
         <v>30</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H10" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
         <v>26</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="4">
         <v>21</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
         <v>28</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E11" s="4">
         <v>12</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F11" s="7">
         <f>25/3.6</f>
         <v>6.9444444444444446</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G11" s="7">
         <v>30</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H11" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
         <v>26</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C12" s="4">
         <v>22</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <v>28</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E12" s="4">
         <v>21</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F12" s="7">
         <f>36*1000/3600</f>
         <v>10</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G12" s="7">
         <v>30</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H12" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
         <v>26</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C13" s="4">
         <v>18</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D13" s="2">
         <v>28</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E13" s="4">
         <v>12</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F13" s="7">
         <f>9*10/3.6</f>
         <v>25</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G13" s="7">
         <v>30</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H13" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
         <v>30</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C14" s="4">
         <v>24</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="2">
         <v>32</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E14" s="4">
         <v>12</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F14" s="7">
         <f>3.6*10/3.6</f>
         <v>10</v>
       </c>
-      <c r="G13" s="7">
-        <v>30</v>
-      </c>
-      <c r="H13" s="7">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="2">
-        <v>26</v>
-      </c>
-      <c r="C14" s="4">
-        <v>18</v>
-      </c>
-      <c r="D14" s="2">
-        <v>28</v>
-      </c>
-      <c r="E14" s="4">
-        <v>12</v>
-      </c>
-      <c r="F14" s="7">
-        <v>36</v>
-      </c>
       <c r="G14" s="7">
         <v>30</v>
       </c>
       <c r="H14" s="7">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="4">
         <v>18</v>
@@ -1880,30 +2415,30 @@
         <v>12</v>
       </c>
       <c r="F15" s="7">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G15" s="7">
         <v>30</v>
       </c>
       <c r="H15" s="7">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
         <v>28</v>
       </c>
-      <c r="B16" s="2">
-        <v>2</v>
-      </c>
       <c r="C16" s="4">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E16" s="4">
-        <v>-18</v>
+        <v>12</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -1917,51 +2452,50 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>-18</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
+        <v>30</v>
+      </c>
+      <c r="H17" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2">
         <v>26</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C18" s="4">
         <v>21</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>28</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E18" s="4">
         <v>12</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F18" s="7">
         <f>20*15/3.6</f>
         <v>83.333333333333329</v>
       </c>
-      <c r="G17" s="7">
-        <v>30</v>
-      </c>
-      <c r="H17" s="7">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="2">
-        <v>26</v>
-      </c>
-      <c r="C18" s="4">
-        <v>21</v>
-      </c>
-      <c r="D18" s="2">
-        <v>28</v>
-      </c>
-      <c r="E18" s="4">
-        <v>12</v>
-      </c>
-      <c r="F18" s="7">
-        <f>36/3.6</f>
-        <v>10</v>
-      </c>
       <c r="G18" s="7">
         <v>30</v>
       </c>
@@ -1971,7 +2505,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2">
         <v>26</v>
@@ -1990,7 +2524,7 @@
         <v>10</v>
       </c>
       <c r="G19" s="7">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H19" s="7">
         <v>60</v>
@@ -1998,7 +2532,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2">
         <v>26</v>
@@ -2013,18 +2547,275 @@
         <v>12</v>
       </c>
       <c r="F20" s="7">
+        <f>36/3.6</f>
+        <v>10</v>
+      </c>
+      <c r="G20" s="7">
+        <v>40</v>
+      </c>
+      <c r="H20" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2">
+        <v>26</v>
+      </c>
+      <c r="C21" s="4">
+        <v>21</v>
+      </c>
+      <c r="D21" s="2">
+        <v>28</v>
+      </c>
+      <c r="E21" s="4">
+        <v>12</v>
+      </c>
+      <c r="F21" s="7">
         <f>30/3.6</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G21" s="7">
         <v>30</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H21" s="7">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F5:F21 F2:F3" unlockedFormula="1"/>
+  </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
+    <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="be70d004-d1e5-4317-a402-eff109a4a2bb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="12" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>